<commit_message>
First Commit - ExtractJobDetails
</commit_message>
<xml_diff>
--- a/input/JobFunctions.xlsx
+++ b/input/JobFunctions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="92">
   <si>
     <t>Job Function</t>
   </si>
@@ -151,6 +151,150 @@
   </si>
   <si>
     <t>Wholesales Trade</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Auditing</t>
+  </si>
+  <si>
+    <t>Taxation</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Secretarial</t>
+  </si>
+  <si>
+    <t>Advertising</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Interior Design</t>
+  </si>
+  <si>
+    <t>Banking</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>Promotions</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>Pharmaceutical</t>
+  </si>
+  <si>
+    <t>Logistics</t>
+  </si>
+  <si>
+    <t>Supply Chain</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Public Relations</t>
+  </si>
+  <si>
+    <t>Medical</t>
+  </si>
+  <si>
+    <t>Therapy Services</t>
+  </si>
+  <si>
+    <t>Personal Care</t>
+  </si>
+  <si>
+    <t>Beauty</t>
+  </si>
+  <si>
+    <t>Public Service</t>
+  </si>
+  <si>
+    <t>Civil Service</t>
+  </si>
+  <si>
+    <t>Purchasing</t>
+  </si>
+  <si>
+    <t>Merchandising</t>
+  </si>
+  <si>
+    <t>Real Estate</t>
+  </si>
+  <si>
+    <t>Property Management</t>
+  </si>
+  <si>
+    <t>Repair</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Retail</t>
+  </si>
+  <si>
+    <t>Sciences</t>
+  </si>
+  <si>
+    <t>Laboratory</t>
+  </si>
+  <si>
+    <t>R&amp;D</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Investigation</t>
+  </si>
+  <si>
+    <t>Telecommunication</t>
+  </si>
+  <si>
+    <t>Travel</t>
+  </si>
+  <si>
+    <t>Tourism</t>
+  </si>
+  <si>
+    <t>Wholesale</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Education</t>
   </si>
 </sst>
 </file>
@@ -468,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A44"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,224 +623,473 @@
     <col min="1" max="1" width="30.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>